<commit_message>
Copiar Especial- ID valores, não formula
</commit_message>
<xml_diff>
--- a/output/Base_PPP.xlsx
+++ b/output/Base_PPP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liviabn\Pictures\Base_PPP\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D00D25B5-16BE-48C1-885F-370E0B0C05A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A1D1C7-16CB-4C10-926B-C4046493D677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -135,30 +135,8 @@
 </comments>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5105" uniqueCount="2409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5106" uniqueCount="2409">
   <si>
     <t>Nome</t>
   </si>
@@ -7835,8 +7813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A331" workbookViewId="0">
+      <selection activeCell="A337" sqref="A337"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -7971,8 +7949,7 @@
       </c>
     </row>
     <row r="2" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" cm="1">
-        <f t="array" ref="A2:A340">ROW(A1:A339)</f>
+      <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -31731,9 +31708,6 @@
       </c>
     </row>
     <row r="340" spans="1:34" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A340">
-        <v>339</v>
-      </c>
       <c r="B340" s="8"/>
       <c r="C340" s="8"/>
       <c r="D340" s="8"/>
@@ -54476,1955 +54450,2044 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{418CBCE0-045C-4E33-9C93-A7BD716367D6}">
-  <dimension ref="A1:A324"/>
+  <dimension ref="A1:A339"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1">
-        <v>1</v>
+      <c r="A1" t="s">
+        <v>2282</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2">
-        <f>A1+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3">
         <f>A2+1</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4">
         <f t="shared" ref="A4:A67" si="0">A3+1</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37">
         <f t="shared" si="0"/>
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39">
         <f t="shared" si="0"/>
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47">
         <f t="shared" si="0"/>
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A55">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A56">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A57">
         <f t="shared" si="0"/>
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A58">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A59">
         <f t="shared" si="0"/>
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A60">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61">
         <f t="shared" si="0"/>
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A62">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A63">
         <f t="shared" si="0"/>
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A64">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A66">
         <f t="shared" si="0"/>
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A67">
         <f t="shared" si="0"/>
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A68">
         <f t="shared" ref="A68:A131" si="1">A67+1</f>
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A69">
         <f t="shared" si="1"/>
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A70">
         <f t="shared" si="1"/>
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A71">
         <f t="shared" si="1"/>
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A72">
         <f t="shared" si="1"/>
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A73">
         <f t="shared" si="1"/>
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A74">
         <f t="shared" si="1"/>
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A75">
         <f t="shared" si="1"/>
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A76">
         <f t="shared" si="1"/>
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A77">
         <f t="shared" si="1"/>
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A78">
         <f t="shared" si="1"/>
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A79">
         <f t="shared" si="1"/>
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A80">
         <f t="shared" si="1"/>
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A81">
         <f t="shared" si="1"/>
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A82">
         <f t="shared" si="1"/>
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A83">
         <f t="shared" si="1"/>
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A84">
         <f t="shared" si="1"/>
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A85">
         <f t="shared" si="1"/>
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A86">
         <f t="shared" si="1"/>
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A87">
         <f t="shared" si="1"/>
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A88">
         <f t="shared" si="1"/>
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A89">
         <f t="shared" si="1"/>
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A90">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A91">
         <f t="shared" si="1"/>
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A92">
         <f t="shared" si="1"/>
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A93">
         <f t="shared" si="1"/>
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A94">
         <f t="shared" si="1"/>
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A95">
         <f t="shared" si="1"/>
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A96">
         <f t="shared" si="1"/>
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A97">
         <f t="shared" si="1"/>
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A98">
         <f t="shared" si="1"/>
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A99">
         <f t="shared" si="1"/>
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A100">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A101">
         <f t="shared" si="1"/>
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A102">
         <f t="shared" si="1"/>
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A103">
         <f t="shared" si="1"/>
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A104">
         <f t="shared" si="1"/>
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A105">
         <f t="shared" si="1"/>
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A106">
         <f t="shared" si="1"/>
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A107">
         <f t="shared" si="1"/>
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A108">
         <f t="shared" si="1"/>
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A109">
         <f t="shared" si="1"/>
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A110">
         <f t="shared" si="1"/>
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A111">
         <f t="shared" si="1"/>
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A112">
         <f t="shared" si="1"/>
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A113">
         <f t="shared" si="1"/>
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A114">
         <f t="shared" si="1"/>
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A115">
         <f t="shared" si="1"/>
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A116">
         <f t="shared" si="1"/>
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A117">
         <f t="shared" si="1"/>
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A118">
         <f t="shared" si="1"/>
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A119">
         <f t="shared" si="1"/>
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A120">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A121">
         <f t="shared" si="1"/>
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A122">
         <f t="shared" si="1"/>
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A123">
         <f t="shared" si="1"/>
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A124">
         <f t="shared" si="1"/>
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A125">
         <f t="shared" si="1"/>
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A126">
         <f t="shared" si="1"/>
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A127">
         <f t="shared" si="1"/>
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A128">
         <f t="shared" si="1"/>
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A129">
         <f t="shared" si="1"/>
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A130">
         <f t="shared" si="1"/>
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A131">
         <f t="shared" si="1"/>
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A132">
         <f t="shared" ref="A132:A195" si="2">A131+1</f>
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A133">
         <f t="shared" si="2"/>
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A134">
         <f t="shared" si="2"/>
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A135">
         <f t="shared" si="2"/>
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A136">
         <f t="shared" si="2"/>
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A137">
         <f t="shared" si="2"/>
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A138">
         <f t="shared" si="2"/>
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A139">
         <f t="shared" si="2"/>
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A140">
         <f t="shared" si="2"/>
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A141">
         <f t="shared" si="2"/>
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A142">
         <f t="shared" si="2"/>
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A143">
         <f t="shared" si="2"/>
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A144">
         <f t="shared" si="2"/>
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A145">
         <f t="shared" si="2"/>
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A146">
         <f t="shared" si="2"/>
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A147">
         <f t="shared" si="2"/>
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A148">
         <f t="shared" si="2"/>
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A149">
         <f t="shared" si="2"/>
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A150">
         <f t="shared" si="2"/>
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A151">
         <f t="shared" si="2"/>
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A152">
         <f t="shared" si="2"/>
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A153">
         <f t="shared" si="2"/>
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A154">
         <f t="shared" si="2"/>
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A155">
         <f t="shared" si="2"/>
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A156">
         <f t="shared" si="2"/>
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A157">
         <f t="shared" si="2"/>
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A158">
         <f t="shared" si="2"/>
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A159">
         <f t="shared" si="2"/>
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A160">
         <f t="shared" si="2"/>
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A161">
         <f t="shared" si="2"/>
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A162">
         <f t="shared" si="2"/>
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A163">
         <f t="shared" si="2"/>
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A164">
         <f t="shared" si="2"/>
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A165">
         <f t="shared" si="2"/>
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A166">
         <f t="shared" si="2"/>
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A167">
         <f t="shared" si="2"/>
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A168">
         <f t="shared" si="2"/>
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A169">
         <f t="shared" si="2"/>
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A170">
         <f t="shared" si="2"/>
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A171">
         <f t="shared" si="2"/>
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A172">
         <f t="shared" si="2"/>
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A173">
         <f t="shared" si="2"/>
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A174">
         <f t="shared" si="2"/>
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A175">
         <f t="shared" si="2"/>
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A176">
         <f t="shared" si="2"/>
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A177">
         <f t="shared" si="2"/>
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A178">
         <f t="shared" si="2"/>
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A179">
         <f t="shared" si="2"/>
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A180">
         <f t="shared" si="2"/>
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A181">
         <f t="shared" si="2"/>
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A182">
         <f t="shared" si="2"/>
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A183">
         <f t="shared" si="2"/>
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A184">
         <f t="shared" si="2"/>
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A185">
         <f t="shared" si="2"/>
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A186">
         <f t="shared" si="2"/>
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A187">
         <f t="shared" si="2"/>
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A188">
         <f t="shared" si="2"/>
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A189">
         <f t="shared" si="2"/>
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A190">
         <f t="shared" si="2"/>
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A191">
         <f t="shared" si="2"/>
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A192">
         <f t="shared" si="2"/>
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A193">
         <f t="shared" si="2"/>
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A194">
         <f t="shared" si="2"/>
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A195">
         <f t="shared" si="2"/>
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A196">
         <f t="shared" ref="A196:A259" si="3">A195+1</f>
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A197">
         <f t="shared" si="3"/>
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A198">
         <f t="shared" si="3"/>
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A199">
         <f t="shared" si="3"/>
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A200">
         <f t="shared" si="3"/>
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A201">
         <f t="shared" si="3"/>
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A202">
         <f t="shared" si="3"/>
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A203">
         <f t="shared" si="3"/>
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A204">
         <f t="shared" si="3"/>
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A205">
         <f t="shared" si="3"/>
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A206">
         <f t="shared" si="3"/>
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A207">
         <f t="shared" si="3"/>
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A208">
         <f t="shared" si="3"/>
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A209">
         <f t="shared" si="3"/>
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A210">
         <f t="shared" si="3"/>
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A211">
         <f t="shared" si="3"/>
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A212">
         <f t="shared" si="3"/>
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A213">
         <f t="shared" si="3"/>
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A214">
         <f t="shared" si="3"/>
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A215">
         <f t="shared" si="3"/>
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A216">
         <f t="shared" si="3"/>
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A217">
         <f t="shared" si="3"/>
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A218">
         <f t="shared" si="3"/>
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A219">
         <f t="shared" si="3"/>
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A220">
         <f t="shared" si="3"/>
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A221">
         <f t="shared" si="3"/>
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A222">
         <f t="shared" si="3"/>
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A223">
         <f t="shared" si="3"/>
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A224">
         <f t="shared" si="3"/>
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A225">
         <f t="shared" si="3"/>
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A226">
         <f t="shared" si="3"/>
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A227">
         <f t="shared" si="3"/>
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A228">
         <f t="shared" si="3"/>
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A229">
         <f t="shared" si="3"/>
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A230">
         <f t="shared" si="3"/>
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A231">
         <f t="shared" si="3"/>
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A232">
         <f t="shared" si="3"/>
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A233">
         <f t="shared" si="3"/>
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A234">
         <f t="shared" si="3"/>
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A235">
         <f t="shared" si="3"/>
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A236">
         <f t="shared" si="3"/>
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A237">
         <f t="shared" si="3"/>
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A238">
         <f t="shared" si="3"/>
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A239">
         <f t="shared" si="3"/>
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A240">
         <f t="shared" si="3"/>
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A241">
         <f t="shared" si="3"/>
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A242">
         <f t="shared" si="3"/>
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A243">
         <f t="shared" si="3"/>
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A244">
         <f t="shared" si="3"/>
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A245">
         <f t="shared" si="3"/>
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A246">
         <f t="shared" si="3"/>
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A247">
         <f t="shared" si="3"/>
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A248">
         <f t="shared" si="3"/>
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A249">
         <f t="shared" si="3"/>
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A250">
         <f t="shared" si="3"/>
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A251">
         <f t="shared" si="3"/>
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A252">
         <f t="shared" si="3"/>
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A253">
         <f t="shared" si="3"/>
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A254">
         <f t="shared" si="3"/>
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A255">
         <f t="shared" si="3"/>
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A256">
         <f t="shared" si="3"/>
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A257">
         <f t="shared" si="3"/>
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A258">
         <f t="shared" si="3"/>
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A259">
         <f t="shared" si="3"/>
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A260">
         <f t="shared" ref="A260:A323" si="4">A259+1</f>
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A261">
         <f t="shared" si="4"/>
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A262">
         <f t="shared" si="4"/>
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A263">
         <f t="shared" si="4"/>
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A264">
         <f t="shared" si="4"/>
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A265">
         <f t="shared" si="4"/>
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A266">
         <f t="shared" si="4"/>
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A267">
         <f t="shared" si="4"/>
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A268">
         <f t="shared" si="4"/>
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A269">
         <f t="shared" si="4"/>
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A270">
         <f t="shared" si="4"/>
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A271">
         <f t="shared" si="4"/>
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A272">
         <f t="shared" si="4"/>
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A273">
         <f t="shared" si="4"/>
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A274">
         <f t="shared" si="4"/>
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A275">
         <f t="shared" si="4"/>
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A276">
         <f t="shared" si="4"/>
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A277">
         <f t="shared" si="4"/>
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A278">
         <f t="shared" si="4"/>
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A279">
         <f t="shared" si="4"/>
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A280">
         <f t="shared" si="4"/>
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A281">
         <f t="shared" si="4"/>
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A282">
         <f t="shared" si="4"/>
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A283">
         <f t="shared" si="4"/>
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A284">
         <f t="shared" si="4"/>
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A285">
         <f t="shared" si="4"/>
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A286">
         <f t="shared" si="4"/>
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A287">
         <f t="shared" si="4"/>
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A288">
         <f t="shared" si="4"/>
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A289">
         <f t="shared" si="4"/>
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A290">
         <f t="shared" si="4"/>
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A291">
         <f t="shared" si="4"/>
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A292">
         <f t="shared" si="4"/>
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A293">
         <f t="shared" si="4"/>
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A294">
         <f t="shared" si="4"/>
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A295">
         <f t="shared" si="4"/>
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A296">
         <f t="shared" si="4"/>
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A297">
         <f t="shared" si="4"/>
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A298">
         <f t="shared" si="4"/>
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A299">
         <f t="shared" si="4"/>
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A300">
         <f t="shared" si="4"/>
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="301" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A301">
         <f t="shared" si="4"/>
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="302" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A302">
         <f t="shared" si="4"/>
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="303" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A303">
         <f t="shared" si="4"/>
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="304" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A304">
         <f t="shared" si="4"/>
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="305" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A305">
         <f t="shared" si="4"/>
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="306" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A306">
         <f t="shared" si="4"/>
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="307" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A307">
         <f t="shared" si="4"/>
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="308" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A308">
         <f t="shared" si="4"/>
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="309" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A309">
         <f t="shared" si="4"/>
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="310" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A310">
         <f t="shared" si="4"/>
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="311" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A311">
         <f t="shared" si="4"/>
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="312" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A312">
         <f t="shared" si="4"/>
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="313" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A313">
         <f t="shared" si="4"/>
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="314" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A314">
         <f t="shared" si="4"/>
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="315" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A315">
         <f t="shared" si="4"/>
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="316" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A316">
         <f t="shared" si="4"/>
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A317">
         <f t="shared" si="4"/>
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="318" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A318">
         <f t="shared" si="4"/>
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="319" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A319">
         <f t="shared" si="4"/>
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="320" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A320">
         <f t="shared" si="4"/>
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="321" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A321">
         <f t="shared" si="4"/>
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="322" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A322">
         <f t="shared" si="4"/>
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="323" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A323">
         <f t="shared" si="4"/>
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="324" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A324">
-        <f t="shared" ref="A324" si="5">A323+1</f>
+        <f t="shared" ref="A324:A339" si="5">A323+1</f>
+        <v>323</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A325">
+        <f t="shared" si="5"/>
         <v>324</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A326">
+        <f t="shared" si="5"/>
+        <v>325</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A327">
+        <f t="shared" si="5"/>
+        <v>326</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A328">
+        <f t="shared" si="5"/>
+        <v>327</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A329">
+        <f t="shared" si="5"/>
+        <v>328</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A330">
+        <f t="shared" si="5"/>
+        <v>329</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A331">
+        <f t="shared" si="5"/>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A332">
+        <f t="shared" si="5"/>
+        <v>331</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A333">
+        <f t="shared" si="5"/>
+        <v>332</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A334">
+        <f t="shared" si="5"/>
+        <v>333</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A335">
+        <f t="shared" si="5"/>
+        <v>334</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A336">
+        <f t="shared" si="5"/>
+        <v>335</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A337">
+        <f t="shared" si="5"/>
+        <v>336</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A338">
+        <f t="shared" si="5"/>
+        <v>337</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A339">
+        <f t="shared" si="5"/>
+        <v>338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>